<commit_message>
An example of how one could implement object handles
</commit_message>
<xml_diff>
--- a/Source/Samples/Registration.Sample/Registration.Samples.xlsx
+++ b/Source/Samples/Registration.Sample/Registration.Samples.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Tests for Complex</t>
   </si>
@@ -79,6 +78,21 @@
   </si>
   <si>
     <t>IEnumerable&lt;Enum&gt;</t>
+  </si>
+  <si>
+    <t>One call returning IEnumerable&lt;T&gt;</t>
+  </si>
+  <si>
+    <t>Multiple calls returning T</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Object handles</t>
   </si>
 </sst>
 </file>
@@ -439,20 +453,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="b">
-        <f>AND(A4:A15)</f>
+        <f>AND(A4:A31)</f>
         <v>1</v>
       </c>
     </row>
@@ -839,6 +856,177 @@
       </c>
       <c r="J20" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="array" ref="D23:D25">_xll.dnaFactoryMultiple(E23:E25,F23:F25)</f>
+        <v>SampleClass1@530</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="str">
+        <f>_xll.dnaFactorySingle(E23,F23)</f>
+        <v>SampleClass1@529</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <v>SampleClass2@531</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="str">
+        <f>_xll.dnaFactorySingle(E24,F24)</f>
+        <v>SampleClass2@539</v>
+      </c>
+      <c r="J24" t="str">
+        <f>_xll.dnaFactoryCompound(G24,G23)</f>
+        <v>Compound@541</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <v>SampleClass1@532</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" t="str">
+        <f>_xll.dnaFactorySingle(E25,F25)</f>
+        <v>SampleClass1@540</v>
+      </c>
+      <c r="J25" t="str">
+        <f>_xll.dnaFactoryCompound(J24,G25)</f>
+        <v>Compound@543</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="b">
+        <f>SUMSQ(B26:C26)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26" si="9">D26-G26</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>G26-J26</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>_xll.dnaUseSomeHandles(D23:D25)</f>
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <f>_xll.dnaUseSomeHandles(G23:G25)</f>
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <f>_xll.dnaUseSomeHandles(J25)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="array" ref="D28:D30">_xll.dnaFactoryMultiple(E28:E30,F28:F30)</f>
+        <v>SampleClass2@535</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28" t="str">
+        <f>_xll.dnaFactorySingle(E28,F28)</f>
+        <v>SampleClass2@533</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D29" t="str">
+        <v>SampleClass1@536</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29" t="str">
+        <f>_xll.dnaFactorySingle(E29,F29)</f>
+        <v>SampleClass1@538</v>
+      </c>
+      <c r="J29" t="str">
+        <f>_xll.dnaFactoryCompound(G29,G28)</f>
+        <v>Compound@542</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <v>SampleClass2@537</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30" t="str">
+        <f>_xll.dnaFactorySingle(E30,F30)</f>
+        <v>SampleClass2@534</v>
+      </c>
+      <c r="J30" t="str">
+        <f>_xll.dnaFactoryCompound(J29,G30)</f>
+        <v>Compound@544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="b">
+        <f>SUMSQ(B31:C31)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ref="B31" si="10">D31-G31</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>G31-J31</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>_xll.dnaUseSomeHandles(D28:D30)</f>
+        <v>57</v>
+      </c>
+      <c r="G31">
+        <f>_xll.dnaUseSomeHandles(G28:G30)</f>
+        <v>57</v>
+      </c>
+      <c r="J31">
+        <f>_xll.dnaUseSomeHandles(J30)</f>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>